<commit_message>
default deserializer - prototyp
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\source\repos\XMLExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03BF3C1-C3C2-4E8E-8E34-C85287E5FCA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7555735B-0A27-4B9F-A02B-36724A96AEDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Czas [h]</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Połączenie się z repo GitLaba, dodano plik Resources.resx dla ścieżek do pliku</t>
+  </si>
+  <si>
+    <t>Razem</t>
   </si>
 </sst>
 </file>
@@ -476,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776B16D4-4A4E-B64F-A019-C52527AB2E2A}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -489,7 +492,7 @@
     <col min="3" max="3" width="101.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -499,8 +502,11 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44013</v>
       </c>
@@ -510,8 +516,12 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>SUM(B:B)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44013</v>
       </c>
@@ -522,7 +532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44014</v>
       </c>
@@ -533,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>44014</v>
       </c>
@@ -544,7 +554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>44015</v>
       </c>
@@ -555,7 +565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>44015</v>
       </c>
@@ -566,7 +576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44017</v>
       </c>
@@ -577,7 +587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>44018</v>
       </c>
@@ -588,7 +598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>44018</v>
       </c>
@@ -599,7 +609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44019</v>
       </c>
@@ -610,7 +620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44020</v>
       </c>
@@ -621,7 +631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44021</v>
       </c>
@@ -632,7 +642,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44021</v>
       </c>
@@ -643,7 +653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44021</v>
       </c>
@@ -660,12 +670,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -801,15 +808,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -833,10 +844,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
zamiania atrybutów w elementy
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\source\repos\XMLExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA8E90C-8B15-492D-A7A9-87C08B3518BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7846A0B8-2903-4F82-98AF-58937FB0F296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Czas [h]</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>DefaultDeserializer + katalogi</t>
+  </si>
+  <si>
+    <t>DefaultSerializer + testy</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776B16D4-4A4E-B64F-A019-C52527AB2E2A}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -521,7 +524,7 @@
       </c>
       <c r="E2">
         <f>SUM(B:B)</f>
-        <v>21.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -676,6 +679,17 @@
       </c>
       <c r="C16" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nowy plik xsl + próby stworzenia dynamicznego xsla
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\source\repos\XMLExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7846A0B8-2903-4F82-98AF-58937FB0F296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0282C947-A6EE-4923-9101-74F8085F6F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Czas [h]</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>DefaultSerializer + testy</t>
+  </si>
+  <si>
+    <t>atrybuty w elementy</t>
+  </si>
+  <si>
+    <t>Próba ogarnięcia XSLT. Ustawianie namespace. Czy jest sens w dynamicznym tworzeniu XSLT dla każdego templatu osobno?</t>
+  </si>
+  <si>
+    <t>Projektowanie rozwiązania problemu dynamicznego XSLT</t>
+  </si>
+  <si>
+    <t>Poprawna nauka XSLT. Nowy plik output.xsl</t>
   </si>
 </sst>
 </file>
@@ -485,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776B16D4-4A4E-B64F-A019-C52527AB2E2A}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -524,7 +536,7 @@
       </c>
       <c r="E2">
         <f>SUM(B:B)</f>
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -690,6 +702,50 @@
       </c>
       <c r="C17" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -704,15 +760,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000FFFA20196C5244A198B956263BCCC6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e665c9909af2d00025ac938ed956f4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65d88d86-0354-4735-9d62-80a4ac60412a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d6152cd73a56170a76ea3621d94087c" ns2:_="">
     <xsd:import namespace="65d88d86-0354-4735-9d62-80a4ac60412a"/>
@@ -844,6 +891,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
   <ds:schemaRefs>
@@ -854,14 +910,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCBFDAD8-0F07-4DA1-82D3-259155DCA012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -877,4 +925,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
prototyp aplikacji konsolowej XSLTransform
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\source\repos\XMLExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0282C947-A6EE-4923-9101-74F8085F6F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB60D47-8A1A-48D0-98C0-4A2AB90D92BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Czas [h]</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Poprawna nauka XSLT. Nowy plik output.xsl</t>
+  </si>
+  <si>
+    <t>Pisanie kolejnego pliku XSL, z łatwo edytowalnymi kolumnami do wybrania</t>
+  </si>
+  <si>
+    <t>Oddzielenie XSLT z głównego projektu do osobnego. Praca nad finalną aplikacją do XSLT.</t>
   </si>
 </sst>
 </file>
@@ -497,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776B16D4-4A4E-B64F-A019-C52527AB2E2A}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -536,7 +542,7 @@
       </c>
       <c r="E2">
         <f>SUM(B:B)</f>
-        <v>27</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -746,6 +752,28 @@
       </c>
       <c r="C21" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -760,6 +788,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000FFFA20196C5244A198B956263BCCC6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e665c9909af2d00025ac938ed956f4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65d88d86-0354-4735-9d62-80a4ac60412a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d6152cd73a56170a76ea3621d94087c" ns2:_="">
     <xsd:import namespace="65d88d86-0354-4735-9d62-80a4ac60412a"/>
@@ -891,15 +928,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
   <ds:schemaRefs>
@@ -910,6 +938,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCBFDAD8-0F07-4DA1-82D3-259155DCA012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -925,12 +961,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aplikacja konsolowa XSLT poprawiona + aplikacja XMLExportH
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\source\repos\XMLExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB60D47-8A1A-48D0-98C0-4A2AB90D92BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A11C985-348E-45FF-88AB-08D50A10AB45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Czas [h]</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Oddzielenie XSLT z głównego projektu do osobnego. Praca nad finalną aplikacją do XSLT.</t>
+  </si>
+  <si>
+    <t>Praca nad poprawnymi aplikacjami konsolowymi.</t>
   </si>
 </sst>
 </file>
@@ -503,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776B16D4-4A4E-B64F-A019-C52527AB2E2A}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -542,7 +545,7 @@
       </c>
       <c r="E2">
         <f>SUM(B:B)</f>
-        <v>29.5</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -774,6 +777,17 @@
       </c>
       <c r="C23" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -788,15 +802,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000FFFA20196C5244A198B956263BCCC6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e665c9909af2d00025ac938ed956f4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65d88d86-0354-4735-9d62-80a4ac60412a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d6152cd73a56170a76ea3621d94087c" ns2:_="">
     <xsd:import namespace="65d88d86-0354-4735-9d62-80a4ac60412a"/>
@@ -928,6 +933,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
   <ds:schemaRefs>
@@ -938,14 +952,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCBFDAD8-0F07-4DA1-82D3-259155DCA012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -961,4 +967,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Nowe testy + Aplikacje konsolowe
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\source\repos\XMLExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A11C985-348E-45FF-88AB-08D50A10AB45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE801FB-2E6E-4CC7-9500-6F0165BA06F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Czas [h]</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Praca nad poprawnymi aplikacjami konsolowymi.</t>
+  </si>
+  <si>
+    <t>Praca nad poprawnymi aplikacjami konsolowymi - dla dynamicznego</t>
+  </si>
+  <si>
+    <t>Uczenie się o testach.</t>
+  </si>
+  <si>
+    <t>Nowe testy</t>
   </si>
 </sst>
 </file>
@@ -506,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776B16D4-4A4E-B64F-A019-C52527AB2E2A}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -545,7 +554,7 @@
       </c>
       <c r="E2">
         <f>SUM(B:B)</f>
-        <v>33.5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -788,6 +797,39 @@
       </c>
       <c r="C24" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>44028</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>44028</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
XSLConstructor v2. outputTemplate jako embedded resource
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\source\repos\XMLExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE801FB-2E6E-4CC7-9500-6F0165BA06F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F25C47A-12E3-4B95-8836-9E5312B8A397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Czas [h]</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Nowe testy</t>
+  </si>
+  <si>
+    <t>XSLConstructor. Embedded resources.</t>
   </si>
 </sst>
 </file>
@@ -515,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776B16D4-4A4E-B64F-A019-C52527AB2E2A}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -554,7 +557,7 @@
       </c>
       <c r="E2">
         <f>SUM(B:B)</f>
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -830,6 +833,17 @@
       </c>
       <c r="C27" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>44028</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -844,6 +858,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000FFFA20196C5244A198B956263BCCC6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e665c9909af2d00025ac938ed956f4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65d88d86-0354-4735-9d62-80a4ac60412a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d6152cd73a56170a76ea3621d94087c" ns2:_="">
     <xsd:import namespace="65d88d86-0354-4735-9d62-80a4ac60412a"/>
@@ -975,15 +998,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
   <ds:schemaRefs>
@@ -994,6 +1008,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCBFDAD8-0F07-4DA1-82D3-259155DCA012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1009,12 +1031,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
prototyp połączonych generic i hcoded projektow
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\source\repos\XMLExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F25C47A-12E3-4B95-8836-9E5312B8A397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F859E31-3357-4F76-AF62-730973791AAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Czas [h]</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>XSLConstructor. Embedded resources.</t>
+  </si>
+  <si>
+    <t>XSLConstructor w osobnym programie</t>
+  </si>
+  <si>
+    <t>RabbitMQ</t>
   </si>
 </sst>
 </file>
@@ -518,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776B16D4-4A4E-B64F-A019-C52527AB2E2A}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -557,7 +563,7 @@
       </c>
       <c r="E2">
         <f>SUM(B:B)</f>
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -844,6 +850,39 @@
       </c>
       <c r="C28" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>44032</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>44032</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>44034</v>
+      </c>
+      <c r="B31" s="1">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -858,15 +897,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000FFFA20196C5244A198B956263BCCC6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e665c9909af2d00025ac938ed956f4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65d88d86-0354-4735-9d62-80a4ac60412a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d6152cd73a56170a76ea3621d94087c" ns2:_="">
     <xsd:import namespace="65d88d86-0354-4735-9d62-80a4ac60412a"/>
@@ -998,6 +1028,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
   <ds:schemaRefs>
@@ -1008,14 +1047,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCBFDAD8-0F07-4DA1-82D3-259155DCA012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1031,4 +1062,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update defaultdeserializer i deserialized element. entity framwork prototyp
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\source\repos\XMLExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D5F455-F9C9-4B10-9541-24D20A81D627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74F1329-72B4-41F5-9E52-AE5EADCB7E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Czas [h]</t>
   </si>
@@ -150,6 +150,12 @@
   <si>
     <t>Query do tabeli z relacją wiele do wielu w SQL. Łączenie się z bazą danych z poziomu C#. Wywoływanie query z poziomu C#. 
 Przeniesienie RabbitReceive na .NetFramework. Prototyp gotowego rozwiązania.</t>
+  </si>
+  <si>
+    <t>internal_value dla XMLExportDC. Upgrade i instalacja VS2019</t>
+  </si>
+  <si>
+    <t>Instalacja ETCore. Budowa modelu istniejącej bazy. Tutoriale do EF.</t>
   </si>
 </sst>
 </file>
@@ -541,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776B16D4-4A4E-B64F-A019-C52527AB2E2A}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -580,7 +586,7 @@
       </c>
       <c r="E2">
         <f>SUM(B:B)</f>
-        <v>62.5</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -955,6 +961,39 @@
       </c>
       <c r="C36" s="5" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>44039</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>44039</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>44039</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -969,15 +1008,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000FFFA20196C5244A198B956263BCCC6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e665c9909af2d00025ac938ed956f4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65d88d86-0354-4735-9d62-80a4ac60412a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d6152cd73a56170a76ea3621d94087c" ns2:_="">
     <xsd:import namespace="65d88d86-0354-4735-9d62-80a4ac60412a"/>
@@ -1109,6 +1139,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
   <ds:schemaRefs>
@@ -1119,14 +1158,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCBFDAD8-0F07-4DA1-82D3-259155DCA012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1142,4 +1173,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
pozbyto się starych projektów
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\source\repos\XMLExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1927D923-5BC5-4590-9A6E-754AD73EBA4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C9AE7D-5190-451D-8EF0-C389F38B41C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Czas [h]</t>
   </si>
@@ -159,6 +159,10 @@
   </si>
   <si>
     <t>Przeniesienia Consumera do EFCore.</t>
+  </si>
+  <si>
+    <t>Nowa tabela bazie stworzona przy użyciu migracji EF. Zmieniona wiadomość wyjątku dodawania do bazy danych. 
+Logowanie czasu dostarczenia raportu i czy został poprawnie dodany. Nowe testy dla XMLExport.</t>
   </si>
 </sst>
 </file>
@@ -550,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776B16D4-4A4E-B64F-A019-C52527AB2E2A}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -589,7 +593,7 @@
       </c>
       <c r="E2">
         <f>SUM(B:B)</f>
-        <v>70.5</v>
+        <v>74.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1008,6 +1012,17 @@
       </c>
       <c r="C40" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B41" s="1">
+        <v>4</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1022,15 +1037,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000FFFA20196C5244A198B956263BCCC6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e665c9909af2d00025ac938ed956f4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65d88d86-0354-4735-9d62-80a4ac60412a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d6152cd73a56170a76ea3621d94087c" ns2:_="">
     <xsd:import namespace="65d88d86-0354-4735-9d62-80a4ac60412a"/>
@@ -1162,6 +1168,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
   <ds:schemaRefs>
@@ -1172,14 +1187,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCBFDAD8-0F07-4DA1-82D3-259155DCA012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1195,4 +1202,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
firebase - dependency event
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\source\repos\XMLExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400A7974-54F7-4ED1-B1DE-0A4ED2119A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9327C796-83EB-498F-AFF7-B105FF8C06A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4485" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{ECB5B274-4C85-A246-9F39-27C65DC5E6A5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Czas [h]</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t>Wysyłanie danych w pętli czasowej. Próba odpalenia singletona na contexcie, nieudana, nie da się bez restrukturyzacji projektu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">przeniesienie modelu do osobnego projektu. Dłubanie nad serwerem iis, niestety </t>
+  </si>
+  <si>
+    <t>firebase</t>
   </si>
 </sst>
 </file>
@@ -579,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776B16D4-4A4E-B64F-A019-C52527AB2E2A}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -618,7 +624,7 @@
       </c>
       <c r="E2">
         <f>SUM(B:B)</f>
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1158,6 +1164,28 @@
       </c>
       <c r="C51" s="5" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1166,21 +1194,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000FFFA20196C5244A198B956263BCCC6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e665c9909af2d00025ac938ed956f4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65d88d86-0354-4735-9d62-80a4ac60412a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d6152cd73a56170a76ea3621d94087c" ns2:_="">
     <xsd:import namespace="65d88d86-0354-4735-9d62-80a4ac60412a"/>
@@ -1312,24 +1325,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCBFDAD8-0F07-4DA1-82D3-259155DCA012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1345,4 +1356,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>